<commit_message>
updates to baseline tables
</commit_message>
<xml_diff>
--- a/BASELINE/20241031.MR_CVD_MDD.AE.CEA.BaselineTable.xlsx
+++ b/BASELINE/20241031.MR_CVD_MDD.AE.CEA.BaselineTable.xlsx
@@ -1,32 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/slaan3/git/CirculatoryHealth/MR_CVD_MDD/BASELINE/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DFC7BA-C4CE-084D-860B-E108F5DBD962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="26180" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="AE_Base_CEA" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="AE_Base_CEA" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="531">
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Missing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="531">
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>Overall</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
   <si>
     <t xml:space="preserve">     2595</t>
@@ -35,10 +43,10 @@
     <t xml:space="preserve">    </t>
   </si>
   <si>
-    <t xml:space="preserve">Hospital....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">St. Antonius, Nieuwegein</t>
+    <t>Hospital....freq.</t>
+  </si>
+  <si>
+    <t>St. Antonius, Nieuwegein</t>
   </si>
   <si>
     <t xml:space="preserve">     36.5 ( 947) </t>
@@ -47,283 +55,283 @@
     <t xml:space="preserve"> 0.0</t>
   </si>
   <si>
-    <t xml:space="preserve">X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UMC Utrecht</t>
+    <t>X</t>
+  </si>
+  <si>
+    <t>UMC Utrecht</t>
   </si>
   <si>
     <t xml:space="preserve">     63.5 (1648) </t>
   </si>
   <si>
-    <t xml:space="preserve">ORyear....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No data available/missing</t>
+    <t>ORyear....freq.</t>
+  </si>
+  <si>
+    <t>No data available/missing</t>
   </si>
   <si>
     <t xml:space="preserve">      0.0 (   0) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2002</t>
+    <t>X.1</t>
+  </si>
+  <si>
+    <t>2002</t>
   </si>
   <si>
     <t xml:space="preserve">      3.1 (  81) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2003</t>
+    <t>X.2</t>
+  </si>
+  <si>
+    <t>2003</t>
   </si>
   <si>
     <t xml:space="preserve">      6.1 ( 157) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2004</t>
+    <t>X.3</t>
+  </si>
+  <si>
+    <t>2004</t>
   </si>
   <si>
     <t xml:space="preserve">      7.3 ( 190) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2005</t>
+    <t>X.4</t>
+  </si>
+  <si>
+    <t>2005</t>
   </si>
   <si>
     <t xml:space="preserve">      7.2 ( 186) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2006</t>
+    <t>X.5</t>
+  </si>
+  <si>
+    <t>2006</t>
   </si>
   <si>
     <t xml:space="preserve">      7.1 ( 183) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2007</t>
+    <t>X.6</t>
+  </si>
+  <si>
+    <t>2007</t>
   </si>
   <si>
     <t xml:space="preserve">      5.9 ( 152) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2008</t>
+    <t>X.7</t>
+  </si>
+  <si>
+    <t>2008</t>
   </si>
   <si>
     <t xml:space="preserve">      5.4 ( 139) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2010</t>
+    <t>X.8</t>
+  </si>
+  <si>
+    <t>2009</t>
+  </si>
+  <si>
+    <t>X.9</t>
+  </si>
+  <si>
+    <t>2010</t>
   </si>
   <si>
     <t xml:space="preserve">      6.1 ( 159) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2011</t>
+    <t>X.10</t>
+  </si>
+  <si>
+    <t>2011</t>
   </si>
   <si>
     <t xml:space="preserve">      6.4 ( 165) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2012</t>
+    <t>X.11</t>
+  </si>
+  <si>
+    <t>2012</t>
   </si>
   <si>
     <t xml:space="preserve">      6.7 ( 174) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2013</t>
+    <t>X.12</t>
+  </si>
+  <si>
+    <t>2013</t>
   </si>
   <si>
     <t xml:space="preserve">      5.7 ( 149) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2014</t>
+    <t>X.13</t>
+  </si>
+  <si>
+    <t>2014</t>
   </si>
   <si>
     <t xml:space="preserve">      6.3 ( 164) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015</t>
+    <t>X.14</t>
+  </si>
+  <si>
+    <t>2015</t>
   </si>
   <si>
     <t xml:space="preserve">      3.0 (  77) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016</t>
+    <t>X.15</t>
+  </si>
+  <si>
+    <t>2016</t>
   </si>
   <si>
     <t xml:space="preserve">      3.3 (  85) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017</t>
+    <t>X.16</t>
+  </si>
+  <si>
+    <t>2017</t>
   </si>
   <si>
     <t xml:space="preserve">      2.5 (  66) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018</t>
+    <t>X.17</t>
+  </si>
+  <si>
+    <t>2018</t>
   </si>
   <si>
     <t xml:space="preserve">      2.7 (  70) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2020</t>
+    <t>X.18</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>X.19</t>
+  </si>
+  <si>
+    <t>2020</t>
   </si>
   <si>
     <t xml:space="preserve">      2.1 (  55) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022</t>
+    <t>X.20</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>X.21</t>
+  </si>
+  <si>
+    <t>2022</t>
   </si>
   <si>
     <t xml:space="preserve">      1.1 (  28) </t>
   </si>
   <si>
-    <t xml:space="preserve">Age..mean..SD..</t>
+    <t>Age..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">   69.242 (9.215)</t>
   </si>
   <si>
-    <t xml:space="preserve">Gender....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">female</t>
+    <t>Gender....freq.</t>
+  </si>
+  <si>
+    <t>female</t>
   </si>
   <si>
     <t xml:space="preserve">     30.5 ( 792) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">male</t>
+    <t>X.22</t>
+  </si>
+  <si>
+    <t>male</t>
   </si>
   <si>
     <t xml:space="preserve">     69.5 (1803) </t>
   </si>
   <si>
-    <t xml:space="preserve">TC_final..mean..SD..</t>
+    <t>TC_final..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">    4.752 (1.436)</t>
   </si>
   <si>
-    <t xml:space="preserve">37.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LDL_final..mean..SD..</t>
+    <t>37.4</t>
+  </si>
+  <si>
+    <t>LDL_final..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">    2.792 (1.220)</t>
   </si>
   <si>
-    <t xml:space="preserve">44.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HDL_final..mean..SD..</t>
+    <t>44.6</t>
+  </si>
+  <si>
+    <t>HDL_final..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">    1.205 (0.433)</t>
   </si>
   <si>
-    <t xml:space="preserve">40.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TG_final..mean..SD..</t>
+    <t>40.8</t>
+  </si>
+  <si>
+    <t>TG_final..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">    1.719 (1.047)</t>
   </si>
   <si>
-    <t xml:space="preserve">41.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">systolic..mean..SD..</t>
+    <t>41.9</t>
+  </si>
+  <si>
+    <t>systolic..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">  151.831 (24.909)</t>
   </si>
   <si>
-    <t xml:space="preserve">10.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diastoli..mean..SD..</t>
+    <t>10.8</t>
+  </si>
+  <si>
+    <t>diastoli..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">   80.959 (24.503)</t>
   </si>
   <si>
-    <t xml:space="preserve">10.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GFR_MDRD..mean..SD..</t>
+    <t>10.9</t>
+  </si>
+  <si>
+    <t>GFR_MDRD..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">   73.806 (21.883)</t>
@@ -332,7 +340,7 @@
     <t xml:space="preserve"> 4.2</t>
   </si>
   <si>
-    <t xml:space="preserve">BMI..mean..SD..</t>
+    <t>BMI..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">   26.525 (4.106)</t>
@@ -341,112 +349,112 @@
     <t xml:space="preserve"> 3.7</t>
   </si>
   <si>
-    <t xml:space="preserve">KDOQI....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Normal kidney function</t>
+    <t>KDOQI....freq.</t>
+  </si>
+  <si>
+    <t>X.23</t>
+  </si>
+  <si>
+    <t>Normal kidney function</t>
   </si>
   <si>
     <t xml:space="preserve">     20.4 ( 529) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CKD 2 (Mild)</t>
+    <t>X.24</t>
+  </si>
+  <si>
+    <t>CKD 2 (Mild)</t>
   </si>
   <si>
     <t xml:space="preserve">     50.9 (1322) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CKD 3 (Moderate)</t>
+    <t>X.25</t>
+  </si>
+  <si>
+    <t>CKD 3 (Moderate)</t>
   </si>
   <si>
     <t xml:space="preserve">     22.9 ( 593) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CKD 4 (Severe)</t>
+    <t>X.26</t>
+  </si>
+  <si>
+    <t>CKD 4 (Severe)</t>
   </si>
   <si>
     <t xml:space="preserve">      1.2 (  32) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CKD 5 (Failure)</t>
+    <t>X.27</t>
+  </si>
+  <si>
+    <t>CKD 5 (Failure)</t>
   </si>
   <si>
     <t xml:space="preserve">      0.4 (  10) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NA</t>
+    <t>X.28</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
   <si>
     <t xml:space="preserve">      4.2 ( 109) </t>
   </si>
   <si>
-    <t xml:space="preserve">BMI_WHO....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Underweight</t>
+    <t>BMI_WHO....freq.</t>
+  </si>
+  <si>
+    <t>X.29</t>
+  </si>
+  <si>
+    <t>Underweight</t>
   </si>
   <si>
     <t xml:space="preserve">      1.0 (  27) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Normal</t>
+    <t>X.30</t>
+  </si>
+  <si>
+    <t>Normal</t>
   </si>
   <si>
     <t xml:space="preserve">     35.9 ( 932) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overweight</t>
+    <t>X.31</t>
+  </si>
+  <si>
+    <t>Overweight</t>
   </si>
   <si>
     <t xml:space="preserve">     43.9 (1140) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Obese</t>
+    <t>X.32</t>
+  </si>
+  <si>
+    <t>Obese</t>
   </si>
   <si>
     <t xml:space="preserve">     15.4 ( 399) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.33</t>
+    <t>X.33</t>
   </si>
   <si>
     <t xml:space="preserve">      3.7 (  97) </t>
   </si>
   <si>
-    <t xml:space="preserve">SmokerStatus....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Current smoker</t>
+    <t>SmokerStatus....freq.</t>
+  </si>
+  <si>
+    <t>Current smoker</t>
   </si>
   <si>
     <t xml:space="preserve">     33.6 ( 873) </t>
@@ -455,34 +463,34 @@
     <t xml:space="preserve"> 4.5</t>
   </si>
   <si>
-    <t xml:space="preserve">X.34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ex-smoker</t>
+    <t>X.34</t>
+  </si>
+  <si>
+    <t>Ex-smoker</t>
   </si>
   <si>
     <t xml:space="preserve">     48.4 (1256) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Never smoked</t>
+    <t>X.35</t>
+  </si>
+  <si>
+    <t>Never smoked</t>
   </si>
   <si>
     <t xml:space="preserve">     13.5 ( 350) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.36</t>
+    <t>X.36</t>
   </si>
   <si>
     <t xml:space="preserve">      4.5 ( 116) </t>
   </si>
   <si>
-    <t xml:space="preserve">AlcoholUse....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
+    <t>AlcoholUse....freq.</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
   <si>
     <t xml:space="preserve">     34.8 ( 904) </t>
@@ -491,25 +499,25 @@
     <t xml:space="preserve"> 3.8</t>
   </si>
   <si>
-    <t xml:space="preserve">X.37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
+    <t>X.37</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
   <si>
     <t xml:space="preserve">     61.4 (1593) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.38</t>
+    <t>X.38</t>
   </si>
   <si>
     <t xml:space="preserve">      3.8 (  98) </t>
   </si>
   <si>
-    <t xml:space="preserve">DiabetesStatus....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Control (no Diabetes Dx/Med)</t>
+    <t>DiabetesStatus....freq.</t>
+  </si>
+  <si>
+    <t>Control (no Diabetes Dx/Med)</t>
   </si>
   <si>
     <t xml:space="preserve">     76.5 (1986) </t>
@@ -518,748 +526,748 @@
     <t xml:space="preserve"> 0.1</t>
   </si>
   <si>
-    <t xml:space="preserve">X.39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diabetes</t>
+    <t>X.39</t>
+  </si>
+  <si>
+    <t>Diabetes</t>
   </si>
   <si>
     <t xml:space="preserve">     23.4 ( 607) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.40</t>
+    <t>X.40</t>
   </si>
   <si>
     <t xml:space="preserve">      0.1 (   2) </t>
   </si>
   <si>
-    <t xml:space="preserve">Hypertension.selfreport....freq.</t>
+    <t>Hypertension.selfreport....freq.</t>
   </si>
   <si>
     <t xml:space="preserve"> 2.2</t>
   </si>
   <si>
-    <t xml:space="preserve">X.41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
+    <t>X.41</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
   <si>
     <t xml:space="preserve">     24.5 ( 635) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yes</t>
+    <t>X.42</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
   <si>
     <t xml:space="preserve">     73.3 (1903) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.43</t>
+    <t>X.43</t>
   </si>
   <si>
     <t xml:space="preserve">      2.2 (  57) </t>
   </si>
   <si>
-    <t xml:space="preserve">Hypertension.selfreportdrug....freq.</t>
+    <t>Hypertension.selfreportdrug....freq.</t>
   </si>
   <si>
     <t xml:space="preserve"> 3.2</t>
   </si>
   <si>
-    <t xml:space="preserve">X.44</t>
+    <t>X.44</t>
   </si>
   <si>
     <t xml:space="preserve">     30.0 ( 779) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.45</t>
+    <t>X.45</t>
   </si>
   <si>
     <t xml:space="preserve">     66.7 (1732) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.46</t>
+    <t>X.46</t>
   </si>
   <si>
     <t xml:space="preserve">      3.2 (  84) </t>
   </si>
   <si>
-    <t xml:space="preserve">Hypertension.composite....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.47</t>
+    <t>Hypertension.composite....freq.</t>
+  </si>
+  <si>
+    <t>X.47</t>
   </si>
   <si>
     <t xml:space="preserve">     14.8 ( 385) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.48</t>
+    <t>X.48</t>
   </si>
   <si>
     <t xml:space="preserve">     85.0 (2207) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.49</t>
+    <t>X.49</t>
   </si>
   <si>
     <t xml:space="preserve">      0.1 (   3) </t>
   </si>
   <si>
-    <t xml:space="preserve">Hypertension.drugs....freq.</t>
+    <t>Hypertension.drugs....freq.</t>
   </si>
   <si>
     <t xml:space="preserve"> 0.5</t>
   </si>
   <si>
-    <t xml:space="preserve">X.50</t>
+    <t>X.50</t>
   </si>
   <si>
     <t xml:space="preserve">     23.5 ( 611) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.51</t>
+    <t>X.51</t>
   </si>
   <si>
     <t xml:space="preserve">     76.0 (1972) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.52</t>
+    <t>X.52</t>
   </si>
   <si>
     <t xml:space="preserve">      0.5 (  12) </t>
   </si>
   <si>
-    <t xml:space="preserve">Med.anticoagulants....freq.</t>
+    <t>Med.anticoagulants....freq.</t>
   </si>
   <si>
     <t xml:space="preserve"> 1.0</t>
   </si>
   <si>
-    <t xml:space="preserve">X.53</t>
+    <t>X.53</t>
   </si>
   <si>
     <t xml:space="preserve">     87.9 (2280) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.54</t>
+    <t>X.54</t>
   </si>
   <si>
     <t xml:space="preserve">     11.1 ( 288) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Med.all.antiplatelet....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.56</t>
+    <t>X.55</t>
+  </si>
+  <si>
+    <t>Med.all.antiplatelet....freq.</t>
+  </si>
+  <si>
+    <t>X.56</t>
   </si>
   <si>
     <t xml:space="preserve">     12.4 ( 322) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.57</t>
+    <t>X.57</t>
   </si>
   <si>
     <t xml:space="preserve">     87.1 (2259) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.58</t>
+    <t>X.58</t>
   </si>
   <si>
     <t xml:space="preserve">      0.5 (  14) </t>
   </si>
   <si>
-    <t xml:space="preserve">Med.Statin.LLD....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.59</t>
+    <t>Med.Statin.LLD....freq.</t>
+  </si>
+  <si>
+    <t>X.59</t>
   </si>
   <si>
     <t xml:space="preserve">     19.7 ( 511) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.60</t>
+    <t>X.60</t>
   </si>
   <si>
     <t xml:space="preserve">     79.8 (2071) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.61</t>
+    <t>X.61</t>
   </si>
   <si>
     <t xml:space="preserve">      0.5 (  13) </t>
   </si>
   <si>
-    <t xml:space="preserve">Stroke_Dx....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No stroke diagnosed</t>
+    <t>Stroke_Dx....freq.</t>
+  </si>
+  <si>
+    <t>X.62</t>
+  </si>
+  <si>
+    <t>No stroke diagnosed</t>
   </si>
   <si>
     <t xml:space="preserve">     73.0 (1894) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stroke diagnosed</t>
+    <t>X.63</t>
+  </si>
+  <si>
+    <t>Stroke diagnosed</t>
   </si>
   <si>
     <t xml:space="preserve">     22.5 ( 584) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.64</t>
+    <t>X.64</t>
   </si>
   <si>
     <t xml:space="preserve">      4.5 ( 117) </t>
   </si>
   <si>
-    <t xml:space="preserve">sympt....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">missing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.65</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asymptomatic</t>
+    <t>sympt....freq.</t>
+  </si>
+  <si>
+    <t>missing</t>
+  </si>
+  <si>
+    <t>X.65</t>
+  </si>
+  <si>
+    <t>Asymptomatic</t>
   </si>
   <si>
     <t xml:space="preserve">     11.0 ( 286) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.66</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TIA</t>
+    <t>X.66</t>
+  </si>
+  <si>
+    <t>TIA</t>
   </si>
   <si>
     <t xml:space="preserve">     39.0 (1011) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.67</t>
-  </si>
-  <si>
-    <t xml:space="preserve">minor stroke</t>
+    <t>X.67</t>
+  </si>
+  <si>
+    <t>minor stroke</t>
   </si>
   <si>
     <t xml:space="preserve">     15.8 ( 410) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.68</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Major stroke</t>
+    <t>X.68</t>
+  </si>
+  <si>
+    <t>Major stroke</t>
   </si>
   <si>
     <t xml:space="preserve">     10.6 ( 276) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.69</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amaurosis fugax</t>
+    <t>X.69</t>
+  </si>
+  <si>
+    <t>Amaurosis fugax</t>
   </si>
   <si>
     <t xml:space="preserve">     15.9 ( 412) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Four vessel disease</t>
+    <t>X.70</t>
+  </si>
+  <si>
+    <t>Four vessel disease</t>
   </si>
   <si>
     <t xml:space="preserve">      1.5 (  38) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.71</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vertebrobasilary TIA</t>
+    <t>X.71</t>
+  </si>
+  <si>
+    <t>Vertebrobasilary TIA</t>
   </si>
   <si>
     <t xml:space="preserve">      0.2 (   5) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.72</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retinal infarction</t>
+    <t>X.72</t>
+  </si>
+  <si>
+    <t>Retinal infarction</t>
   </si>
   <si>
     <t xml:space="preserve">      1.4 (  37) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.73</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Symptomatic, but aspecific symtoms</t>
+    <t>X.73</t>
+  </si>
+  <si>
+    <t>Symptomatic, but aspecific symtoms</t>
   </si>
   <si>
     <t xml:space="preserve">      2.2 (  56) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.74</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contralateral symptomatic occlusion</t>
+    <t>X.74</t>
+  </si>
+  <si>
+    <t>Contralateral symptomatic occlusion</t>
   </si>
   <si>
     <t xml:space="preserve">      0.4 (  11) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">retinal infarction</t>
+    <t>X.75</t>
+  </si>
+  <si>
+    <t>retinal infarction</t>
   </si>
   <si>
     <t xml:space="preserve">      0.3 (   9) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.76</t>
-  </si>
-  <si>
-    <t xml:space="preserve">armclaudication due to occlusion subclavian artery, CEA needed for bypass</t>
+    <t>X.76</t>
+  </si>
+  <si>
+    <t>armclaudication due to occlusion subclavian artery, CEA needed for bypass</t>
   </si>
   <si>
     <t xml:space="preserve">      0.0 (   1) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.77</t>
-  </si>
-  <si>
-    <t xml:space="preserve">retinal infarction + TIAs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.78</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ocular ischemic syndrome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.79</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ischemisch glaucoom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">subclavian steal syndrome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.81</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TGA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.82</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Symptoms.5G....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.83</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ocular</t>
+    <t>X.77</t>
+  </si>
+  <si>
+    <t>retinal infarction + TIAs</t>
+  </si>
+  <si>
+    <t>X.78</t>
+  </si>
+  <si>
+    <t>Ocular ischemic syndrome</t>
+  </si>
+  <si>
+    <t>X.79</t>
+  </si>
+  <si>
+    <t>ischemisch glaucoom</t>
+  </si>
+  <si>
+    <t>X.80</t>
+  </si>
+  <si>
+    <t>subclavian steal syndrome</t>
+  </si>
+  <si>
+    <t>X.81</t>
+  </si>
+  <si>
+    <t>TGA</t>
+  </si>
+  <si>
+    <t>X.82</t>
+  </si>
+  <si>
+    <t>Symptoms.5G....freq.</t>
+  </si>
+  <si>
+    <t>X.83</t>
+  </si>
+  <si>
+    <t>Ocular</t>
   </si>
   <si>
     <t xml:space="preserve">     16.9 ( 439) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.84</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other</t>
+    <t>X.84</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
   <si>
     <t xml:space="preserve">      4.2 ( 108) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.85</t>
+    <t>X.85</t>
   </si>
   <si>
     <t xml:space="preserve">      1.8 (  46) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.86</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stroke</t>
+    <t>X.86</t>
+  </si>
+  <si>
+    <t>Stroke</t>
   </si>
   <si>
     <t xml:space="preserve">     26.4 ( 686) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.87</t>
+    <t>X.87</t>
   </si>
   <si>
     <t xml:space="preserve">     39.2 (1017) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.88</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AsymptSympt....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.89</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ocular and others</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.90</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Symptomatic</t>
+    <t>X.88</t>
+  </si>
+  <si>
+    <t>AsymptSympt....freq.</t>
+  </si>
+  <si>
+    <t>X.89</t>
+  </si>
+  <si>
+    <t>Ocular and others</t>
+  </si>
+  <si>
+    <t>X.90</t>
+  </si>
+  <si>
+    <t>Symptomatic</t>
   </si>
   <si>
     <t xml:space="preserve">     65.6 (1703) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.91</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AsymptSympt2G....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.92</t>
+    <t>X.91</t>
+  </si>
+  <si>
+    <t>AsymptSympt2G....freq.</t>
+  </si>
+  <si>
+    <t>X.92</t>
   </si>
   <si>
     <t xml:space="preserve">     88.5 (2296) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.93</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Symptoms.Update2G....freq.</t>
+    <t>X.93</t>
+  </si>
+  <si>
+    <t>Symptoms.Update2G....freq.</t>
   </si>
   <si>
     <t xml:space="preserve">     26.1 ( 676) </t>
   </si>
   <si>
-    <t xml:space="preserve">17.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.94</t>
+    <t>17.5</t>
+  </si>
+  <si>
+    <t>X.94</t>
   </si>
   <si>
     <t xml:space="preserve">     56.5 (1465) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.95</t>
+    <t>X.95</t>
   </si>
   <si>
     <t xml:space="preserve">     17.5 ( 454) </t>
   </si>
   <si>
-    <t xml:space="preserve">Symptoms.Update3G....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.96</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.97</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unclear</t>
+    <t>Symptoms.Update3G....freq.</t>
+  </si>
+  <si>
+    <t>14.6</t>
+  </si>
+  <si>
+    <t>X.96</t>
+  </si>
+  <si>
+    <t>X.97</t>
+  </si>
+  <si>
+    <t>Unclear</t>
   </si>
   <si>
     <t xml:space="preserve">      2.9 (  76) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.98</t>
+    <t>X.98</t>
   </si>
   <si>
     <t xml:space="preserve">     14.6 ( 378) </t>
   </si>
   <si>
-    <t xml:space="preserve">restenos....freq.</t>
+    <t>restenos....freq.</t>
   </si>
   <si>
     <t xml:space="preserve"> 1.4</t>
   </si>
   <si>
-    <t xml:space="preserve">X.99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">de novo</t>
+    <t>X.99</t>
+  </si>
+  <si>
+    <t>de novo</t>
   </si>
   <si>
     <t xml:space="preserve">     93.6 (2428) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">restenosis</t>
+    <t>X.100</t>
+  </si>
+  <si>
+    <t>restenosis</t>
   </si>
   <si>
     <t xml:space="preserve">      5.0 ( 130) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stenose bij angioseal na PTCA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.102</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stenose....freq.</t>
+    <t>X.101</t>
+  </si>
+  <si>
+    <t>stenose bij angioseal na PTCA</t>
+  </si>
+  <si>
+    <t>X.102</t>
+  </si>
+  <si>
+    <t>stenose....freq.</t>
   </si>
   <si>
     <t xml:space="preserve"> 2.0</t>
   </si>
   <si>
-    <t xml:space="preserve">X.103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-49%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.104</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50-70%</t>
+    <t>X.103</t>
+  </si>
+  <si>
+    <t>0-49%</t>
+  </si>
+  <si>
+    <t>X.104</t>
+  </si>
+  <si>
+    <t>50-70%</t>
   </si>
   <si>
     <t xml:space="preserve">      8.1 ( 210) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.105</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70-90%</t>
+    <t>X.105</t>
+  </si>
+  <si>
+    <t>70-90%</t>
   </si>
   <si>
     <t xml:space="preserve">     45.9 (1192) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.106</t>
-  </si>
-  <si>
-    <t xml:space="preserve">90-99%</t>
+    <t>X.106</t>
+  </si>
+  <si>
+    <t>90-99%</t>
   </si>
   <si>
     <t xml:space="preserve">     37.9 ( 983) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.107</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100% (Occlusion)</t>
+    <t>X.107</t>
+  </si>
+  <si>
+    <t>100% (Occlusion)</t>
   </si>
   <si>
     <t xml:space="preserve">      1.3 (  35) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.108</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.109</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50-99%</t>
+    <t>X.108</t>
+  </si>
+  <si>
+    <t>X.109</t>
+  </si>
+  <si>
+    <t>50-99%</t>
   </si>
   <si>
     <t xml:space="preserve">      0.7 (  18) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.110</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70-99%</t>
+    <t>X.110</t>
+  </si>
+  <si>
+    <t>70-99%</t>
   </si>
   <si>
     <t xml:space="preserve">      3.5 (  90) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.111</t>
-  </si>
-  <si>
-    <t xml:space="preserve">99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.112</t>
+    <t>X.111</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>X.112</t>
   </si>
   <si>
     <t xml:space="preserve">      2.0 (  51) </t>
   </si>
   <si>
-    <t xml:space="preserve">Artery_summary....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No artery known (yet), no surgery (patient ill, died, exited study), re-numbered to AAA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.113</t>
-  </si>
-  <si>
-    <t xml:space="preserve">carotid (left &amp; right)</t>
+    <t>Artery_summary....freq.</t>
+  </si>
+  <si>
+    <t>No artery known (yet), no surgery (patient ill, died, exited study), re-numbered to AAA</t>
+  </si>
+  <si>
+    <t>X.113</t>
+  </si>
+  <si>
+    <t>carotid (left &amp; right)</t>
   </si>
   <si>
     <t xml:space="preserve">     98.3 (2551) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.114</t>
-  </si>
-  <si>
-    <t xml:space="preserve">femoral/iliac (left, right or both sides)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.115</t>
-  </si>
-  <si>
-    <t xml:space="preserve">other carotid arteries (common, external)</t>
+    <t>X.114</t>
+  </si>
+  <si>
+    <t>femoral/iliac (left, right or both sides)</t>
+  </si>
+  <si>
+    <t>X.115</t>
+  </si>
+  <si>
+    <t>other carotid arteries (common, external)</t>
   </si>
   <si>
     <t xml:space="preserve">      1.7 (  44) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.116</t>
-  </si>
-  <si>
-    <t xml:space="preserve">carotid bypass and injury (left, right or both sides)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.117</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aneurysmata (carotid &amp; femoral)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.118</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aorta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.119</t>
-  </si>
-  <si>
-    <t xml:space="preserve">other arteries (renal, popliteal, vertebral)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.120</t>
-  </si>
-  <si>
-    <t xml:space="preserve">femoral bypass, angioseal and injury (left, right or both sides)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAD_history....freq.</t>
+    <t>X.116</t>
+  </si>
+  <si>
+    <t>carotid bypass and injury (left, right or both sides)</t>
+  </si>
+  <si>
+    <t>X.117</t>
+  </si>
+  <si>
+    <t>aneurysmata (carotid &amp; femoral)</t>
+  </si>
+  <si>
+    <t>X.118</t>
+  </si>
+  <si>
+    <t>aorta</t>
+  </si>
+  <si>
+    <t>X.119</t>
+  </si>
+  <si>
+    <t>other arteries (renal, popliteal, vertebral)</t>
+  </si>
+  <si>
+    <t>X.120</t>
+  </si>
+  <si>
+    <t>femoral bypass, angioseal and injury (left, right or both sides)</t>
+  </si>
+  <si>
+    <t>CAD_history....freq.</t>
   </si>
   <si>
     <t xml:space="preserve"> 0.2</t>
   </si>
   <si>
-    <t xml:space="preserve">X.121</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No history CAD</t>
+    <t>X.121</t>
+  </si>
+  <si>
+    <t>No history CAD</t>
   </si>
   <si>
     <t xml:space="preserve">     68.1 (1768) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.122</t>
-  </si>
-  <si>
-    <t xml:space="preserve">History CAD</t>
+    <t>X.122</t>
+  </si>
+  <si>
+    <t>History CAD</t>
   </si>
   <si>
     <t xml:space="preserve">     31.7 ( 822) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAOD....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">missing/no data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.124</t>
+    <t>X.123</t>
+  </si>
+  <si>
+    <t>PAOD....freq.</t>
+  </si>
+  <si>
+    <t>missing/no data</t>
+  </si>
+  <si>
+    <t>X.124</t>
   </si>
   <si>
     <t xml:space="preserve">     78.8 (2045) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.125</t>
+    <t>X.125</t>
   </si>
   <si>
     <t xml:space="preserve">     21.0 ( 546) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.126</t>
+    <t>X.126</t>
   </si>
   <si>
     <t xml:space="preserve">      0.2 (   4) </t>
   </si>
   <si>
-    <t xml:space="preserve">Peripheral.interv....freq.</t>
+    <t>Peripheral.interv....freq.</t>
   </si>
   <si>
     <t xml:space="preserve">     78.5 (2038) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.127</t>
+    <t>X.127</t>
   </si>
   <si>
     <t xml:space="preserve">     21.0 ( 544) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EP_composite....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No data available.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.129</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No composite endpoints</t>
+    <t>X.128</t>
+  </si>
+  <si>
+    <t>EP_composite....freq.</t>
+  </si>
+  <si>
+    <t>No data available.</t>
+  </si>
+  <si>
+    <t>X.129</t>
+  </si>
+  <si>
+    <t>No composite endpoints</t>
   </si>
   <si>
     <t xml:space="preserve">     72.2 (1873) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.130</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Composite endpoints</t>
+    <t>X.130</t>
+  </si>
+  <si>
+    <t>Composite endpoints</t>
   </si>
   <si>
     <t xml:space="preserve">     25.6 ( 665) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.131</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EP_composite_time..mean..SD..</t>
+    <t>X.131</t>
+  </si>
+  <si>
+    <t>EP_composite_time..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">    9.614 (357.762)</t>
@@ -1268,193 +1276,193 @@
     <t xml:space="preserve"> 2.3</t>
   </si>
   <si>
-    <t xml:space="preserve">EP_major....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.132</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No major events (endpoints)</t>
+    <t>EP_major....freq.</t>
+  </si>
+  <si>
+    <t>X.132</t>
+  </si>
+  <si>
+    <t>No major events (endpoints)</t>
   </si>
   <si>
     <t xml:space="preserve">     85.4 (2217) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.133</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Major events (endpoints)</t>
+    <t>X.133</t>
+  </si>
+  <si>
+    <t>Major events (endpoints)</t>
   </si>
   <si>
     <t xml:space="preserve">     12.4 ( 321) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.134</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EP_major_time..mean..SD..</t>
+    <t>X.134</t>
+  </si>
+  <si>
+    <t>EP_major_time..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">    9.857 (357.757)</t>
   </si>
   <si>
-    <t xml:space="preserve">MAC_rankNorm..mean..SD..</t>
+    <t>MAC_rankNorm..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">    0.178 (0.952)</t>
   </si>
   <si>
-    <t xml:space="preserve">34.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMC_rankNorm..mean..SD..</t>
+    <t>34.3</t>
+  </si>
+  <si>
+    <t>SMC_rankNorm..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">   -0.061 (0.962)</t>
   </si>
   <si>
-    <t xml:space="preserve">34.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Macrophages.bin....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no/minor</t>
+    <t>34.4</t>
+  </si>
+  <si>
+    <t>Macrophages.bin....freq.</t>
+  </si>
+  <si>
+    <t>no/minor</t>
   </si>
   <si>
     <t xml:space="preserve">     37.5 ( 974) </t>
   </si>
   <si>
-    <t xml:space="preserve">13.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.135</t>
-  </si>
-  <si>
-    <t xml:space="preserve">moderate/heavy</t>
+    <t>13.9</t>
+  </si>
+  <si>
+    <t>X.135</t>
+  </si>
+  <si>
+    <t>moderate/heavy</t>
   </si>
   <si>
     <t xml:space="preserve">     48.5 (1259) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.136</t>
+    <t>X.136</t>
   </si>
   <si>
     <t xml:space="preserve">     13.9 ( 362) </t>
   </si>
   <si>
-    <t xml:space="preserve">SMC.bin....freq.</t>
+    <t>SMC.bin....freq.</t>
   </si>
   <si>
     <t xml:space="preserve">     29.2 ( 759) </t>
   </si>
   <si>
-    <t xml:space="preserve">13.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.137</t>
+    <t>13.6</t>
+  </si>
+  <si>
+    <t>X.137</t>
   </si>
   <si>
     <t xml:space="preserve">     57.2 (1484) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.138</t>
+    <t>X.138</t>
   </si>
   <si>
     <t xml:space="preserve">     13.6 ( 352) </t>
   </si>
   <si>
-    <t xml:space="preserve">Neutrophils_rankNorm..mean..SD..</t>
+    <t>Neutrophils_rankNorm..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">    0.027 (0.951)</t>
   </si>
   <si>
-    <t xml:space="preserve">88.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MastCells_rankNorm..mean..SD..</t>
+    <t>88.2</t>
+  </si>
+  <si>
+    <t>MastCells_rankNorm..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">   -0.010 (1.002)</t>
   </si>
   <si>
-    <t xml:space="preserve">90.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IPH.bin....freq.</t>
+    <t>90.7</t>
+  </si>
+  <si>
+    <t>IPH.bin....freq.</t>
   </si>
   <si>
     <t xml:space="preserve">     33.5 ( 870) </t>
   </si>
   <si>
-    <t xml:space="preserve">13.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.139</t>
+    <t>13.3</t>
+  </si>
+  <si>
+    <t>X.139</t>
   </si>
   <si>
     <t xml:space="preserve">     53.1 (1379) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.140</t>
+    <t>X.140</t>
   </si>
   <si>
     <t xml:space="preserve">     13.3 ( 346) </t>
   </si>
   <si>
-    <t xml:space="preserve">VesselDensity_rankNorm..mean..SD..</t>
+    <t>VesselDensity_rankNorm..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">    0.057 (0.983)</t>
   </si>
   <si>
-    <t xml:space="preserve">39.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calc.bin....freq.</t>
+    <t>39.4</t>
+  </si>
+  <si>
+    <t>Calc.bin....freq.</t>
   </si>
   <si>
     <t xml:space="preserve">     48.9 (1270) </t>
   </si>
   <si>
-    <t xml:space="preserve">11.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.141</t>
+    <t>11.8</t>
+  </si>
+  <si>
+    <t>X.141</t>
   </si>
   <si>
     <t xml:space="preserve">     39.3 (1020) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.142</t>
+    <t>X.142</t>
   </si>
   <si>
     <t xml:space="preserve">     11.8 ( 305) </t>
   </si>
   <si>
-    <t xml:space="preserve">Collagen.bin....freq.</t>
+    <t>Collagen.bin....freq.</t>
   </si>
   <si>
     <t xml:space="preserve">     16.8 ( 436) </t>
   </si>
   <si>
-    <t xml:space="preserve">20.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.143</t>
+    <t>20.8</t>
+  </si>
+  <si>
+    <t>X.143</t>
   </si>
   <si>
     <t xml:space="preserve">     62.4 (1619) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.144</t>
+    <t>X.144</t>
   </si>
   <si>
     <t xml:space="preserve">     20.8 ( 540) </t>
   </si>
   <si>
-    <t xml:space="preserve">Fat.bin_10....freq.</t>
+    <t>Fat.bin_10....freq.</t>
   </si>
   <si>
     <t xml:space="preserve"> &lt;10%</t>
@@ -1463,10 +1471,10 @@
     <t xml:space="preserve">     25.2 ( 654) </t>
   </si>
   <si>
-    <t xml:space="preserve">11.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.145</t>
+    <t>11.7</t>
+  </si>
+  <si>
+    <t>X.145</t>
   </si>
   <si>
     <t xml:space="preserve"> &gt;10%</t>
@@ -1475,133 +1483,133 @@
     <t xml:space="preserve">     63.1 (1637) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.146</t>
+    <t>X.146</t>
   </si>
   <si>
     <t xml:space="preserve">     11.7 ( 304) </t>
   </si>
   <si>
-    <t xml:space="preserve">Fat.bin_40....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;40%</t>
+    <t>Fat.bin_40....freq.</t>
+  </si>
+  <si>
+    <t>&lt;40%</t>
   </si>
   <si>
     <t xml:space="preserve">     63.3 (1642) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.147</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&gt;40%</t>
+    <t>X.147</t>
+  </si>
+  <si>
+    <t>&gt;40%</t>
   </si>
   <si>
     <t xml:space="preserve">     25.0 ( 649) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.148</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OverallPlaquePhenotype....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">atheromatous</t>
+    <t>X.148</t>
+  </si>
+  <si>
+    <t>OverallPlaquePhenotype....freq.</t>
+  </si>
+  <si>
+    <t>atheromatous</t>
   </si>
   <si>
     <t xml:space="preserve">     24.4 ( 632) </t>
   </si>
   <si>
-    <t xml:space="preserve">12.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.149</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fibroatheromatous</t>
+    <t>12.1</t>
+  </si>
+  <si>
+    <t>X.149</t>
+  </si>
+  <si>
+    <t>fibroatheromatous</t>
   </si>
   <si>
     <t xml:space="preserve">     32.4 ( 841) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fibrous</t>
+    <t>X.150</t>
+  </si>
+  <si>
+    <t>fibrous</t>
   </si>
   <si>
     <t xml:space="preserve">     31.2 ( 809) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.151</t>
+    <t>X.151</t>
   </si>
   <si>
     <t xml:space="preserve">     12.1 ( 313) </t>
   </si>
   <si>
-    <t xml:space="preserve">Plaque_Vulnerability_Index....freq.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0</t>
+    <t>Plaque_Vulnerability_Index....freq.</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
   <si>
     <t xml:space="preserve">     18.9 ( 490) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.152</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
+    <t>X.152</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
   <si>
     <t xml:space="preserve">     16.3 ( 423) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.153</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
+    <t>X.153</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
   <si>
     <t xml:space="preserve">     21.9 ( 569) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.154</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
+    <t>X.154</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
   <si>
     <t xml:space="preserve">     25.4 ( 658) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.155</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
+    <t>X.155</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
   <si>
     <t xml:space="preserve">     13.1 ( 340) </t>
   </si>
   <si>
-    <t xml:space="preserve">X.156</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
+    <t>X.156</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
   <si>
     <t xml:space="preserve">      4.4 ( 115) </t>
   </si>
   <si>
-    <t xml:space="preserve">PCSK9_plasma..mean..SD..</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32011.795 (18862.086)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">57.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCSK9_plasma_rankNorm..mean..SD..</t>
+    <t>PCSK9_plasma..mean..SD..</t>
+  </si>
+  <si>
+    <t>32011.795 (18862.086)</t>
+  </si>
+  <si>
+    <t>57.6</t>
+  </si>
+  <si>
+    <t>PCSK9_plasma_rankNorm..mean..SD..</t>
   </si>
   <si>
     <t xml:space="preserve">   -0.003 (1.016)</t>
@@ -1611,8 +1619,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1648,6 +1655,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1929,14 +1945,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D216"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C212" sqref="C212"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1950,7 +1974,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1964,7 +1988,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1978,7 +2002,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1992,7 +2016,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2006,7 +2030,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -2020,7 +2044,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2034,7 +2058,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -2048,7 +2072,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -2062,7 +2086,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -2076,7 +2100,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -2090,7 +2114,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -2104,7 +2128,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -2118,7 +2142,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -2132,7 +2156,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -2146,7 +2170,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -2160,7 +2184,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -2174,7 +2198,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -2188,7 +2212,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -2202,7 +2226,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -2216,7 +2240,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -2230,7 +2254,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -2244,7 +2268,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -2258,7 +2282,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -2272,7 +2296,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -2286,7 +2310,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -2300,7 +2324,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>77</v>
       </c>
@@ -2314,7 +2338,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>79</v>
       </c>
@@ -2328,7 +2352,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -2342,7 +2366,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -2356,7 +2380,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -2370,7 +2394,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>91</v>
       </c>
@@ -2384,7 +2408,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>94</v>
       </c>
@@ -2398,7 +2422,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>97</v>
       </c>
@@ -2412,7 +2436,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>100</v>
       </c>
@@ -2426,7 +2450,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>103</v>
       </c>
@@ -2440,7 +2464,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>106</v>
       </c>
@@ -2454,7 +2478,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>109</v>
       </c>
@@ -2468,7 +2492,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>110</v>
       </c>
@@ -2482,7 +2506,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>113</v>
       </c>
@@ -2496,7 +2520,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>116</v>
       </c>
@@ -2510,7 +2534,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>119</v>
       </c>
@@ -2524,7 +2548,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>122</v>
       </c>
@@ -2538,7 +2562,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>125</v>
       </c>
@@ -2552,7 +2576,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>128</v>
       </c>
@@ -2566,7 +2590,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>129</v>
       </c>
@@ -2580,7 +2604,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>132</v>
       </c>
@@ -2594,7 +2618,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>135</v>
       </c>
@@ -2608,7 +2632,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>138</v>
       </c>
@@ -2622,7 +2646,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>141</v>
       </c>
@@ -2636,7 +2660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>143</v>
       </c>
@@ -2650,7 +2674,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>147</v>
       </c>
@@ -2664,7 +2688,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>150</v>
       </c>
@@ -2678,7 +2702,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>153</v>
       </c>
@@ -2692,7 +2716,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>155</v>
       </c>
@@ -2706,7 +2730,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>159</v>
       </c>
@@ -2720,7 +2744,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>162</v>
       </c>
@@ -2734,7 +2758,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>164</v>
       </c>
@@ -2748,7 +2772,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>168</v>
       </c>
@@ -2762,7 +2786,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>171</v>
       </c>
@@ -2776,7 +2800,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>173</v>
       </c>
@@ -2790,7 +2814,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>175</v>
       </c>
@@ -2804,7 +2828,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>178</v>
       </c>
@@ -2818,7 +2842,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>181</v>
       </c>
@@ -2832,7 +2856,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>183</v>
       </c>
@@ -2846,7 +2870,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>185</v>
       </c>
@@ -2860,7 +2884,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>187</v>
       </c>
@@ -2874,7 +2898,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>189</v>
       </c>
@@ -2888,7 +2912,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>191</v>
       </c>
@@ -2902,7 +2926,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>192</v>
       </c>
@@ -2916,7 +2940,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>194</v>
       </c>
@@ -2930,7 +2954,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>196</v>
       </c>
@@ -2944,7 +2968,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>198</v>
       </c>
@@ -2958,7 +2982,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>200</v>
       </c>
@@ -2972,7 +2996,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>202</v>
       </c>
@@ -2986,7 +3010,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>204</v>
       </c>
@@ -3000,7 +3024,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>206</v>
       </c>
@@ -3014,7 +3038,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>208</v>
       </c>
@@ -3028,7 +3052,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>210</v>
       </c>
@@ -3042,7 +3066,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>212</v>
       </c>
@@ -3056,7 +3080,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>213</v>
       </c>
@@ -3070,7 +3094,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>214</v>
       </c>
@@ -3084,7 +3108,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>216</v>
       </c>
@@ -3098,7 +3122,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>218</v>
       </c>
@@ -3112,7 +3136,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>220</v>
       </c>
@@ -3126,7 +3150,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>221</v>
       </c>
@@ -3140,7 +3164,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>223</v>
       </c>
@@ -3154,7 +3178,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>225</v>
       </c>
@@ -3168,7 +3192,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>227</v>
       </c>
@@ -3182,7 +3206,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>228</v>
       </c>
@@ -3196,7 +3220,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>231</v>
       </c>
@@ -3210,7 +3234,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>234</v>
       </c>
@@ -3224,7 +3248,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>236</v>
       </c>
@@ -3238,7 +3262,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>238</v>
       </c>
@@ -3252,7 +3276,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>241</v>
       </c>
@@ -3266,7 +3290,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>244</v>
       </c>
@@ -3280,7 +3304,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>247</v>
       </c>
@@ -3294,7 +3318,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>250</v>
       </c>
@@ -3308,7 +3332,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>253</v>
       </c>
@@ -3322,7 +3346,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>256</v>
       </c>
@@ -3336,7 +3360,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>259</v>
       </c>
@@ -3350,7 +3374,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>262</v>
       </c>
@@ -3364,7 +3388,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>265</v>
       </c>
@@ -3378,7 +3402,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>268</v>
       </c>
@@ -3392,7 +3416,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>271</v>
       </c>
@@ -3406,7 +3430,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>274</v>
       </c>
@@ -3420,7 +3444,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>276</v>
       </c>
@@ -3434,7 +3458,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>278</v>
       </c>
@@ -3448,7 +3472,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>280</v>
       </c>
@@ -3462,7 +3486,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>282</v>
       </c>
@@ -3476,7 +3500,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>284</v>
       </c>
@@ -3490,7 +3514,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>285</v>
       </c>
@@ -3504,7 +3528,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>286</v>
       </c>
@@ -3518,7 +3542,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>289</v>
       </c>
@@ -3532,7 +3556,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>292</v>
       </c>
@@ -3546,7 +3570,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>294</v>
       </c>
@@ -3560,7 +3584,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>297</v>
       </c>
@@ -3574,7 +3598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>299</v>
       </c>
@@ -3588,7 +3612,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>300</v>
       </c>
@@ -3602,7 +3626,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>301</v>
       </c>
@@ -3616,7 +3640,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>303</v>
       </c>
@@ -3630,7 +3654,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>306</v>
       </c>
@@ -3644,7 +3668,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>307</v>
       </c>
@@ -3658,7 +3682,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="124">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>308</v>
       </c>
@@ -3672,7 +3696,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>310</v>
       </c>
@@ -3686,7 +3710,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>311</v>
       </c>
@@ -3700,7 +3724,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="127">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>314</v>
       </c>
@@ -3714,7 +3738,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>316</v>
       </c>
@@ -3728,7 +3752,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>318</v>
       </c>
@@ -3742,7 +3766,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>320</v>
       </c>
@@ -3756,7 +3780,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>321</v>
       </c>
@@ -3770,7 +3794,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="132">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>324</v>
       </c>
@@ -3784,7 +3808,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>326</v>
       </c>
@@ -3798,7 +3822,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>328</v>
       </c>
@@ -3812,7 +3836,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>331</v>
       </c>
@@ -3826,7 +3850,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="136">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>334</v>
       </c>
@@ -3840,7 +3864,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>336</v>
       </c>
@@ -3854,7 +3878,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="138">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>337</v>
       </c>
@@ -3868,7 +3892,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="139">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>339</v>
       </c>
@@ -3882,7 +3906,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="140">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>341</v>
       </c>
@@ -3896,7 +3920,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>344</v>
       </c>
@@ -3910,7 +3934,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>347</v>
       </c>
@@ -3924,7 +3948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>350</v>
       </c>
@@ -3938,7 +3962,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>353</v>
       </c>
@@ -3952,7 +3976,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="145">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>354</v>
       </c>
@@ -3966,7 +3990,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="146">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>357</v>
       </c>
@@ -3980,7 +4004,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>360</v>
       </c>
@@ -3994,7 +4018,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>362</v>
       </c>
@@ -4008,7 +4032,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>364</v>
       </c>
@@ -4022,7 +4046,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="150">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>366</v>
       </c>
@@ -4036,7 +4060,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>369</v>
       </c>
@@ -4050,7 +4074,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>371</v>
       </c>
@@ -4064,7 +4088,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="153">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>374</v>
       </c>
@@ -4078,7 +4102,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="154">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>376</v>
       </c>
@@ -4092,7 +4116,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="155">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>378</v>
       </c>
@@ -4106,7 +4130,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="156">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>380</v>
       </c>
@@ -4120,7 +4144,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="157">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>382</v>
       </c>
@@ -4134,7 +4158,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="158">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>384</v>
       </c>
@@ -4148,7 +4172,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="159">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>386</v>
       </c>
@@ -4162,7 +4186,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="160">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>389</v>
       </c>
@@ -4176,7 +4200,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="161">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>392</v>
       </c>
@@ -4190,7 +4214,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>393</v>
       </c>
@@ -4204,7 +4228,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="163">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>395</v>
       </c>
@@ -4218,7 +4242,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="164">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>397</v>
       </c>
@@ -4232,7 +4256,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="165">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>399</v>
       </c>
@@ -4246,7 +4270,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="166">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>401</v>
       </c>
@@ -4260,7 +4284,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="167">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>403</v>
       </c>
@@ -4274,7 +4298,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="168">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>405</v>
       </c>
@@ -4288,7 +4312,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="169">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>406</v>
       </c>
@@ -4302,7 +4326,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="170">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>408</v>
       </c>
@@ -4316,7 +4340,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="171">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>411</v>
       </c>
@@ -4330,7 +4354,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="172">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>414</v>
       </c>
@@ -4344,7 +4368,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="173">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>415</v>
       </c>
@@ -4358,7 +4382,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="174">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>418</v>
       </c>
@@ -4372,7 +4396,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="175">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>419</v>
       </c>
@@ -4386,7 +4410,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="176">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>422</v>
       </c>
@@ -4400,7 +4424,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="177">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>425</v>
       </c>
@@ -4414,7 +4438,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="178">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>426</v>
       </c>
@@ -4428,7 +4452,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="179">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>428</v>
       </c>
@@ -4442,7 +4466,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="180">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>431</v>
       </c>
@@ -4456,7 +4480,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="181">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>434</v>
       </c>
@@ -4470,7 +4494,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="182">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>438</v>
       </c>
@@ -4484,7 +4508,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="183">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>441</v>
       </c>
@@ -4498,7 +4522,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="184">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>443</v>
       </c>
@@ -4512,7 +4536,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="185">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>446</v>
       </c>
@@ -4526,7 +4550,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="186">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>448</v>
       </c>
@@ -4540,7 +4564,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="187">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>450</v>
       </c>
@@ -4554,7 +4578,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="188">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>453</v>
       </c>
@@ -4568,7 +4592,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="189">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>456</v>
       </c>
@@ -4582,7 +4606,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="190">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>459</v>
       </c>
@@ -4596,7 +4620,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="191">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>461</v>
       </c>
@@ -4610,7 +4634,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="192">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>463</v>
       </c>
@@ -4624,7 +4648,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="193">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>466</v>
       </c>
@@ -4638,7 +4662,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="194">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>469</v>
       </c>
@@ -4652,7 +4676,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="195">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>471</v>
       </c>
@@ -4666,7 +4690,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="196">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>473</v>
       </c>
@@ -4680,7 +4704,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="197">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>476</v>
       </c>
@@ -4694,7 +4718,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="198">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>478</v>
       </c>
@@ -4708,7 +4732,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="199">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>480</v>
       </c>
@@ -4722,7 +4746,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="200">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>484</v>
       </c>
@@ -4736,7 +4760,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="201">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>487</v>
       </c>
@@ -4750,7 +4774,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="202">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>489</v>
       </c>
@@ -4764,7 +4788,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="203">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>492</v>
       </c>
@@ -4778,7 +4802,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="204">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>495</v>
       </c>
@@ -4792,7 +4816,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="205">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>496</v>
       </c>
@@ -4806,7 +4830,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="206">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>500</v>
       </c>
@@ -4820,7 +4844,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="207">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>503</v>
       </c>
@@ -4834,7 +4858,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="208">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>506</v>
       </c>
@@ -4848,7 +4872,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="209">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>508</v>
       </c>
@@ -4862,7 +4886,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="210">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>511</v>
       </c>
@@ -4876,7 +4900,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="211">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>514</v>
       </c>
@@ -4890,7 +4914,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="212">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>517</v>
       </c>
@@ -4904,7 +4928,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="213">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>520</v>
       </c>
@@ -4918,7 +4942,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="214">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>523</v>
       </c>
@@ -4932,7 +4956,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="215">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>526</v>
       </c>
@@ -4946,7 +4970,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="216">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>529</v>
       </c>
@@ -4962,6 +4986,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>